<commit_message>
Zusammenfassung der bachelorarbeit und aktuelle Urlaubsanträge
</commit_message>
<xml_diff>
--- a/Urlaub/Urlaub Brückentag 26.5.2017.xlsx
+++ b/Urlaub/Urlaub Brückentag 26.5.2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7710" yWindow="1650" windowWidth="14940" windowHeight="9150" activeTab="1"/>
+    <workbookView xWindow="-330" yWindow="960" windowWidth="14940" windowHeight="9150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="7" r:id="rId1"/>
@@ -1007,11 +1007,20 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1030,21 +1039,6 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1073,50 +1067,11 @@
     <xf numFmtId="0" fontId="25" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1127,30 +1082,44 @@
     <xf numFmtId="165" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1204,28 +1173,59 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2396,7 +2396,7 @@
   <dimension ref="A1:AJ37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:G21"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2448,14 +2448,14 @@
     </row>
     <row r="2" spans="1:36" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
       <c r="H2" s="11"/>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
@@ -2473,18 +2473,18 @@
       <c r="V2" s="11"/>
       <c r="W2" s="11"/>
       <c r="X2" s="7"/>
-      <c r="Z2" s="93" t="s">
+      <c r="Z2" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="AA2" s="94"/>
-      <c r="AB2" s="94"/>
-      <c r="AC2" s="94"/>
-      <c r="AD2" s="94"/>
-      <c r="AE2" s="94"/>
-      <c r="AF2" s="94"/>
-      <c r="AG2" s="94"/>
-      <c r="AH2" s="94"/>
-      <c r="AI2" s="94"/>
+      <c r="AA2" s="87"/>
+      <c r="AB2" s="87"/>
+      <c r="AC2" s="87"/>
+      <c r="AD2" s="87"/>
+      <c r="AE2" s="87"/>
+      <c r="AF2" s="87"/>
+      <c r="AG2" s="87"/>
+      <c r="AH2" s="87"/>
+      <c r="AI2" s="87"/>
       <c r="AJ2" s="10" t="e">
         <f>IF(#REF!+#REF!+#REF!+#REF!+#REF!=5,4,0)</f>
         <v>#REF!</v>
@@ -2529,14 +2529,14 @@
     </row>
     <row r="4" spans="1:36" s="4" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
       <c r="H4" s="11"/>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
@@ -2568,21 +2568,21 @@
     </row>
     <row r="5" spans="1:36" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
       <c r="H5" s="11"/>
-      <c r="J5" s="87" t="str">
+      <c r="J5" s="105" t="str">
         <f>IF($E$21&lt;&gt;"",IF(AND($E$21="Vollzeit",OR($E$7="",$E$9="",$E$19="",$E$11="",$E$13="")),"Bitte füllen Sie alle rot markierten Felder aus!",IF(AND($E$21="Teilzeit",OR($E$7="",$E$9="",$E$19="",$E$11="",$E$13="",$E$28="",$E$30="",$E$32="",$E$34="",$E$36="")),"Bitte füllen Sie alle rot markierten Felder aus!","Bitte beachten Sie das Tabellenblatt 'Urlaubsantrag'")),"Bitte füllen Sie alle rot markierten Felder aus!")</f>
         <v>Bitte beachten Sie das Tabellenblatt 'Urlaubsantrag'</v>
       </c>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="87"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="105"/>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
@@ -2610,28 +2610,28 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="105"/>
+      <c r="M6" s="105"/>
+      <c r="N6" s="105"/>
     </row>
     <row r="7" spans="1:36" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="89"/>
+      <c r="C7" s="92"/>
       <c r="D7" s="38"/>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="F7" s="102"/>
-      <c r="G7" s="103"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="105"/>
+      <c r="N7" s="105"/>
     </row>
     <row r="8" spans="1:36" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B8" s="36"/>
@@ -2642,16 +2642,16 @@
       <c r="G8" s="39"/>
     </row>
     <row r="9" spans="1:36" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="89"/>
+      <c r="C9" s="92"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="101" t="s">
+      <c r="E9" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="102"/>
-      <c r="G9" s="103"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="101"/>
     </row>
     <row r="10" spans="1:36" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="69"/>
@@ -2665,16 +2665,16 @@
       <c r="Q10" s="80"/>
     </row>
     <row r="11" spans="1:36" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="89"/>
+      <c r="C11" s="92"/>
       <c r="D11" s="36"/>
-      <c r="E11" s="90">
-        <v>19</v>
-      </c>
-      <c r="F11" s="91"/>
-      <c r="G11" s="92"/>
+      <c r="E11" s="93">
+        <v>17</v>
+      </c>
+      <c r="F11" s="94"/>
+      <c r="G11" s="95"/>
       <c r="H11" s="83" t="str">
         <f>IF(Start!$E$21&lt;&gt;"",IF(Start!$E$21="Vollzeit","Tage",IF(Start!$E$21="Teilzeit","Stunden","")),"")</f>
         <v>Tage</v>
@@ -2683,36 +2683,36 @@
       <c r="J11" s="81"/>
     </row>
     <row r="12" spans="1:36" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="103" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="105"/>
+      <c r="C12" s="103"/>
       <c r="D12" s="36"/>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
       <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:36" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="88" t="s">
+      <c r="B13" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="89"/>
+      <c r="C13" s="92"/>
       <c r="D13" s="36"/>
-      <c r="E13" s="90">
+      <c r="E13" s="93">
         <v>5</v>
       </c>
-      <c r="F13" s="91"/>
-      <c r="G13" s="92"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="95"/>
       <c r="H13" s="83" t="str">
         <f>IF(Start!$E$21&lt;&gt;"",IF(Start!$E$21="Vollzeit","Tage",IF(Start!$E$21="Teilzeit","Stunden","")),"")</f>
         <v>Tage</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="102" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="104"/>
+      <c r="C14" s="102"/>
       <c r="E14" s="80"/>
       <c r="F14" s="80"/>
       <c r="G14" s="80"/>
@@ -2725,25 +2725,25 @@
       <c r="G15" s="80"/>
     </row>
     <row r="16" spans="1:36" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
       <c r="H16" s="36"/>
       <c r="I16" s="36"/>
       <c r="J16" s="36"/>
     </row>
     <row r="17" spans="2:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="98"/>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
     </row>
     <row r="18" spans="2:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="14"/>
@@ -2755,15 +2755,15 @@
       <c r="J18" s="80"/>
     </row>
     <row r="19" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="100"/>
-      <c r="E19" s="101" t="s">
+      <c r="C19" s="98"/>
+      <c r="E19" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="102"/>
-      <c r="G19" s="103"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="101"/>
     </row>
     <row r="20" spans="2:10" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="E20" s="13"/>
@@ -2771,15 +2771,15 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="99" t="s">
+      <c r="B21" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="C21" s="100"/>
-      <c r="E21" s="101" t="s">
+      <c r="C21" s="98"/>
+      <c r="E21" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="102"/>
-      <c r="G21" s="103"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="101"/>
     </row>
     <row r="22" spans="2:10" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2808,14 +2808,14 @@
       <c r="J25" s="36"/>
     </row>
     <row r="26" spans="2:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="96" t="s">
+      <c r="B26" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="97"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
       <c r="H26" s="41"/>
       <c r="I26" s="36"/>
       <c r="J26" s="36"/>
@@ -2832,16 +2832,16 @@
       <c r="J27" s="36"/>
     </row>
     <row r="28" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="88" t="s">
+      <c r="B28" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="89"/>
+      <c r="C28" s="92"/>
       <c r="D28" s="43">
         <v>4</v>
       </c>
-      <c r="E28" s="90"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="92"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="95"/>
       <c r="H28" s="36"/>
       <c r="I28" s="36"/>
       <c r="J28" s="36"/>
@@ -2858,16 +2858,16 @@
       <c r="J29" s="36"/>
     </row>
     <row r="30" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="88" t="s">
+      <c r="B30" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="89"/>
+      <c r="C30" s="92"/>
       <c r="D30" s="43">
         <v>4</v>
       </c>
-      <c r="E30" s="90"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="92"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="95"/>
       <c r="H30" s="36"/>
       <c r="I30" s="36"/>
       <c r="J30" s="36"/>
@@ -2884,16 +2884,16 @@
       <c r="J31" s="36"/>
     </row>
     <row r="32" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="88" t="s">
+      <c r="B32" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="89"/>
+      <c r="C32" s="92"/>
       <c r="D32" s="43">
         <v>4</v>
       </c>
-      <c r="E32" s="90"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="92"/>
+      <c r="E32" s="93"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="95"/>
       <c r="H32" s="36"/>
       <c r="I32" s="36"/>
       <c r="J32" s="36"/>
@@ -2910,16 +2910,16 @@
       <c r="J33" s="36"/>
     </row>
     <row r="34" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="88" t="s">
+      <c r="B34" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="89"/>
+      <c r="C34" s="92"/>
       <c r="D34" s="43">
         <v>4</v>
       </c>
-      <c r="E34" s="90"/>
-      <c r="F34" s="91"/>
-      <c r="G34" s="92"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="95"/>
       <c r="H34" s="36"/>
       <c r="I34" s="36"/>
       <c r="J34" s="36"/>
@@ -2936,16 +2936,16 @@
       <c r="J35" s="36"/>
     </row>
     <row r="36" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="88" t="s">
+      <c r="B36" s="91" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="89"/>
+      <c r="C36" s="92"/>
       <c r="D36" s="43">
         <v>4</v>
       </c>
-      <c r="E36" s="90"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="92"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="95"/>
       <c r="H36" s="36"/>
       <c r="I36" s="36"/>
       <c r="J36" s="36"/>
@@ -2964,6 +2964,20 @@
   </sheetData>
   <sheetProtection password="EBDE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="30">
+    <mergeCell ref="J5:N7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E32:G32"/>
     <mergeCell ref="Z2:AI2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B26:G26"/>
@@ -2979,21 +2993,7 @@
     <mergeCell ref="E7:G7"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E32:G32"/>
     <mergeCell ref="B4:G5"/>
-    <mergeCell ref="J5:N7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:G11"/>
   </mergeCells>
   <conditionalFormatting sqref="AJ2:AJ5">
     <cfRule type="cellIs" dxfId="49" priority="20" operator="equal">
@@ -3085,8 +3085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29:AA29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12:V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3158,86 +3158,86 @@
     </row>
     <row r="2" spans="1:51" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="32"/>
-      <c r="B2" s="115" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="115"/>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
-      <c r="AA2" s="115"/>
+      <c r="B2" s="140" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="140"/>
+      <c r="N2" s="140"/>
+      <c r="O2" s="140"/>
+      <c r="P2" s="140"/>
+      <c r="Q2" s="140"/>
+      <c r="R2" s="140"/>
+      <c r="S2" s="140"/>
+      <c r="T2" s="140"/>
+      <c r="U2" s="140"/>
+      <c r="V2" s="140"/>
+      <c r="W2" s="140"/>
+      <c r="X2" s="140"/>
+      <c r="Y2" s="140"/>
+      <c r="Z2" s="140"/>
+      <c r="AA2" s="140"/>
       <c r="AB2" s="34"/>
-      <c r="AD2" s="115"/>
-      <c r="AE2" s="115"/>
-      <c r="AF2" s="115"/>
-      <c r="AG2" s="115"/>
-      <c r="AH2" s="115"/>
-      <c r="AI2" s="115"/>
-      <c r="AJ2" s="115"/>
-      <c r="AK2" s="115"/>
-      <c r="AL2" s="115"/>
-      <c r="AM2" s="115"/>
+      <c r="AD2" s="140"/>
+      <c r="AE2" s="140"/>
+      <c r="AF2" s="140"/>
+      <c r="AG2" s="140"/>
+      <c r="AH2" s="140"/>
+      <c r="AI2" s="140"/>
+      <c r="AJ2" s="140"/>
+      <c r="AK2" s="140"/>
+      <c r="AL2" s="140"/>
+      <c r="AM2" s="140"/>
     </row>
     <row r="3" spans="1:51" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32"/>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
-      <c r="H3" s="115"/>
-      <c r="I3" s="115"/>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="115"/>
-      <c r="N3" s="115"/>
-      <c r="O3" s="115"/>
-      <c r="P3" s="115"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="115"/>
-      <c r="S3" s="115"/>
-      <c r="T3" s="115"/>
-      <c r="U3" s="115"/>
-      <c r="V3" s="115"/>
-      <c r="W3" s="115"/>
-      <c r="X3" s="115"/>
-      <c r="Y3" s="115"/>
-      <c r="Z3" s="115"/>
-      <c r="AA3" s="115"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+      <c r="N3" s="140"/>
+      <c r="O3" s="140"/>
+      <c r="P3" s="140"/>
+      <c r="Q3" s="140"/>
+      <c r="R3" s="140"/>
+      <c r="S3" s="140"/>
+      <c r="T3" s="140"/>
+      <c r="U3" s="140"/>
+      <c r="V3" s="140"/>
+      <c r="W3" s="140"/>
+      <c r="X3" s="140"/>
+      <c r="Y3" s="140"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="140"/>
       <c r="AB3" s="34"/>
       <c r="AC3" s="44"/>
-      <c r="AD3" s="115"/>
-      <c r="AE3" s="115"/>
-      <c r="AF3" s="115"/>
-      <c r="AG3" s="115"/>
-      <c r="AH3" s="115"/>
-      <c r="AI3" s="115"/>
-      <c r="AJ3" s="115"/>
-      <c r="AK3" s="115"/>
-      <c r="AL3" s="115"/>
-      <c r="AM3" s="115"/>
+      <c r="AD3" s="140"/>
+      <c r="AE3" s="140"/>
+      <c r="AF3" s="140"/>
+      <c r="AG3" s="140"/>
+      <c r="AH3" s="140"/>
+      <c r="AI3" s="140"/>
+      <c r="AJ3" s="140"/>
+      <c r="AK3" s="140"/>
+      <c r="AL3" s="140"/>
+      <c r="AM3" s="140"/>
     </row>
     <row r="4" spans="1:51" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="32"/>
@@ -3309,19 +3309,19 @@
       <c r="Z5" s="35"/>
       <c r="AA5" s="35"/>
       <c r="AB5" s="34"/>
-      <c r="AD5" s="111" t="str">
+      <c r="AD5" s="137" t="str">
         <f ca="1">IF(SUM(AN13:AN34)=4,"Druckbar","Noch nicht druckbar!")</f>
         <v>Druckbar</v>
       </c>
-      <c r="AE5" s="111"/>
-      <c r="AF5" s="111"/>
-      <c r="AG5" s="111"/>
-      <c r="AH5" s="111"/>
-      <c r="AI5" s="111"/>
-      <c r="AJ5" s="111"/>
-      <c r="AK5" s="111"/>
-      <c r="AL5" s="111"/>
-      <c r="AM5" s="111"/>
+      <c r="AE5" s="137"/>
+      <c r="AF5" s="137"/>
+      <c r="AG5" s="137"/>
+      <c r="AH5" s="137"/>
+      <c r="AI5" s="137"/>
+      <c r="AJ5" s="137"/>
+      <c r="AK5" s="137"/>
+      <c r="AL5" s="137"/>
+      <c r="AM5" s="137"/>
     </row>
     <row r="6" spans="1:51" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32"/>
@@ -3352,62 +3352,62 @@
       <c r="Z6" s="35"/>
       <c r="AA6" s="35"/>
       <c r="AB6" s="34"/>
-      <c r="AD6" s="111"/>
-      <c r="AE6" s="111"/>
-      <c r="AF6" s="111"/>
-      <c r="AG6" s="111"/>
-      <c r="AH6" s="111"/>
-      <c r="AI6" s="111"/>
-      <c r="AJ6" s="111"/>
-      <c r="AK6" s="111"/>
-      <c r="AL6" s="111"/>
-      <c r="AM6" s="111"/>
+      <c r="AD6" s="137"/>
+      <c r="AE6" s="137"/>
+      <c r="AF6" s="137"/>
+      <c r="AG6" s="137"/>
+      <c r="AH6" s="137"/>
+      <c r="AI6" s="137"/>
+      <c r="AJ6" s="137"/>
+      <c r="AK6" s="137"/>
+      <c r="AL6" s="137"/>
+      <c r="AM6" s="137"/>
     </row>
     <row r="7" spans="1:51" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="32"/>
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="144" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="125" t="str">
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="146" t="str">
         <f>CONCATENATE(Start!E9,", ",Start!E7)</f>
         <v>Schneider, Martin</v>
       </c>
-      <c r="L7" s="125"/>
-      <c r="M7" s="125"/>
-      <c r="N7" s="125"/>
-      <c r="O7" s="125"/>
-      <c r="P7" s="125"/>
-      <c r="Q7" s="125"/>
-      <c r="R7" s="125"/>
-      <c r="S7" s="125"/>
-      <c r="T7" s="125"/>
-      <c r="U7" s="125"/>
-      <c r="V7" s="125"/>
-      <c r="W7" s="125"/>
-      <c r="X7" s="125"/>
-      <c r="Y7" s="125"/>
-      <c r="Z7" s="125"/>
-      <c r="AA7" s="126"/>
+      <c r="L7" s="146"/>
+      <c r="M7" s="146"/>
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="146"/>
+      <c r="R7" s="146"/>
+      <c r="S7" s="146"/>
+      <c r="T7" s="146"/>
+      <c r="U7" s="146"/>
+      <c r="V7" s="146"/>
+      <c r="W7" s="146"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
+      <c r="Z7" s="146"/>
+      <c r="AA7" s="147"/>
       <c r="AB7" s="34"/>
       <c r="AC7" s="44"/>
-      <c r="AD7" s="111"/>
-      <c r="AE7" s="111"/>
-      <c r="AF7" s="111"/>
-      <c r="AG7" s="111"/>
-      <c r="AH7" s="111"/>
-      <c r="AI7" s="111"/>
-      <c r="AJ7" s="111"/>
-      <c r="AK7" s="111"/>
-      <c r="AL7" s="111"/>
-      <c r="AM7" s="111"/>
+      <c r="AD7" s="137"/>
+      <c r="AE7" s="137"/>
+      <c r="AF7" s="137"/>
+      <c r="AG7" s="137"/>
+      <c r="AH7" s="137"/>
+      <c r="AI7" s="137"/>
+      <c r="AJ7" s="137"/>
+      <c r="AK7" s="137"/>
+      <c r="AL7" s="137"/>
+      <c r="AM7" s="137"/>
     </row>
     <row r="8" spans="1:51" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A8" s="32"/>
@@ -3438,68 +3438,68 @@
       <c r="Z8" s="35"/>
       <c r="AA8" s="35"/>
       <c r="AB8" s="34"/>
-      <c r="AD8" s="107" t="s">
+      <c r="AD8" s="151" t="s">
         <v>85</v>
       </c>
-      <c r="AE8" s="107"/>
-      <c r="AF8" s="107"/>
-      <c r="AG8" s="107"/>
-      <c r="AH8" s="107"/>
-      <c r="AI8" s="107"/>
-      <c r="AJ8" s="107"/>
-      <c r="AK8" s="107"/>
-      <c r="AL8" s="107"/>
-      <c r="AM8" s="107"/>
+      <c r="AE8" s="151"/>
+      <c r="AF8" s="151"/>
+      <c r="AG8" s="151"/>
+      <c r="AH8" s="151"/>
+      <c r="AI8" s="151"/>
+      <c r="AJ8" s="151"/>
+      <c r="AK8" s="151"/>
+      <c r="AL8" s="151"/>
+      <c r="AM8" s="151"/>
     </row>
     <row r="9" spans="1:51" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="32"/>
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="124"/>
-      <c r="D9" s="124"/>
-      <c r="E9" s="124"/>
-      <c r="F9" s="127">
+      <c r="C9" s="145"/>
+      <c r="D9" s="145"/>
+      <c r="E9" s="145"/>
+      <c r="F9" s="114">
         <f>IF(AND(K16&lt;&gt;"",R16&lt;&gt;""),IF(YEAR(K16)=YEAR(R16),YEAR(K16),CONCATENATE(YEAR(K16),"/",YEAR(R16))),IF(OR(K16&lt;&gt;"",R16&lt;&gt;""),IF(K16&lt;&gt;"",YEAR(K16),YEAR(R16)),""))</f>
         <v>2017</v>
       </c>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="127"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
       <c r="J9" s="45"/>
-      <c r="K9" s="127" t="s">
+      <c r="K9" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="127"/>
-      <c r="M9" s="127"/>
-      <c r="N9" s="127"/>
-      <c r="O9" s="127"/>
-      <c r="P9" s="127"/>
-      <c r="Q9" s="127"/>
-      <c r="R9" s="128" t="str">
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="114"/>
+      <c r="P9" s="114"/>
+      <c r="Q9" s="114"/>
+      <c r="R9" s="148" t="str">
         <f>IF(AND(K16&lt;&gt;"",R16&lt;&gt;""),IF(MONTH(K16)=MONTH(R16),VLOOKUP(MONTH(K16),Monate!A1:B12,2,FALSE),CONCATENATE(VLOOKUP(MONTH(K16),Monate!A1:B12,2,FALSE),"/",VLOOKUP(MONTH(R16),Monate!A1:B12,2,FALSE))),IF(OR(K16&lt;&gt;"",R16&lt;&gt;""),IF(K16&lt;&gt;"",VLOOKUP(MONTH(K16),Monate!A1:B12,2,FALSE),VLOOKUP(MONTH(R16),Monate!A1:B12,2,FALSE)),""))</f>
         <v>MAI</v>
       </c>
-      <c r="S9" s="128"/>
-      <c r="T9" s="128"/>
-      <c r="U9" s="128"/>
-      <c r="V9" s="128"/>
-      <c r="W9" s="128"/>
-      <c r="X9" s="128"/>
-      <c r="Y9" s="128"/>
-      <c r="Z9" s="128"/>
-      <c r="AA9" s="129"/>
+      <c r="S9" s="148"/>
+      <c r="T9" s="148"/>
+      <c r="U9" s="148"/>
+      <c r="V9" s="148"/>
+      <c r="W9" s="148"/>
+      <c r="X9" s="148"/>
+      <c r="Y9" s="148"/>
+      <c r="Z9" s="148"/>
+      <c r="AA9" s="149"/>
       <c r="AB9" s="34"/>
-      <c r="AD9" s="107"/>
-      <c r="AE9" s="107"/>
-      <c r="AF9" s="107"/>
-      <c r="AG9" s="107"/>
-      <c r="AH9" s="107"/>
-      <c r="AI9" s="107"/>
-      <c r="AJ9" s="107"/>
-      <c r="AK9" s="107"/>
-      <c r="AL9" s="107"/>
-      <c r="AM9" s="107"/>
+      <c r="AD9" s="151"/>
+      <c r="AE9" s="151"/>
+      <c r="AF9" s="151"/>
+      <c r="AG9" s="151"/>
+      <c r="AH9" s="151"/>
+      <c r="AI9" s="151"/>
+      <c r="AJ9" s="151"/>
+      <c r="AK9" s="151"/>
+      <c r="AL9" s="151"/>
+      <c r="AM9" s="151"/>
     </row>
     <row r="10" spans="1:51" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A10" s="32"/>
@@ -3530,39 +3530,39 @@
       <c r="Z10" s="35"/>
       <c r="AA10" s="35"/>
       <c r="AB10" s="34"/>
-      <c r="AD10" s="107"/>
-      <c r="AE10" s="107"/>
-      <c r="AF10" s="107"/>
-      <c r="AG10" s="107"/>
-      <c r="AH10" s="107"/>
-      <c r="AI10" s="107"/>
-      <c r="AJ10" s="107"/>
-      <c r="AK10" s="107"/>
-      <c r="AL10" s="107"/>
-      <c r="AM10" s="107"/>
+      <c r="AD10" s="151"/>
+      <c r="AE10" s="151"/>
+      <c r="AF10" s="151"/>
+      <c r="AG10" s="151"/>
+      <c r="AH10" s="151"/>
+      <c r="AI10" s="151"/>
+      <c r="AJ10" s="151"/>
+      <c r="AK10" s="151"/>
+      <c r="AL10" s="151"/>
+      <c r="AM10" s="151"/>
     </row>
     <row r="11" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="46"/>
-      <c r="K11" s="150" t="s">
+      <c r="K11" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="150"/>
-      <c r="M11" s="150"/>
-      <c r="N11" s="150"/>
-      <c r="O11" s="150"/>
+      <c r="L11" s="120"/>
+      <c r="M11" s="120"/>
+      <c r="N11" s="120"/>
+      <c r="O11" s="120"/>
       <c r="Q11" s="47"/>
-      <c r="R11" s="113" t="s">
+      <c r="R11" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="S11" s="113"/>
-      <c r="T11" s="113"/>
-      <c r="U11" s="113"/>
-      <c r="V11" s="113"/>
-      <c r="Y11" s="150" t="s">
+      <c r="S11" s="119"/>
+      <c r="T11" s="119"/>
+      <c r="U11" s="119"/>
+      <c r="V11" s="119"/>
+      <c r="Y11" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="Z11" s="150"/>
-      <c r="AA11" s="150"/>
+      <c r="Z11" s="120"/>
+      <c r="AA11" s="120"/>
       <c r="AB11" s="34"/>
       <c r="AD11" s="48"/>
       <c r="AE11" s="48"/>
@@ -3580,38 +3580,38 @@
     </row>
     <row r="12" spans="1:51" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="46"/>
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="89"/>
-      <c r="K12" s="147">
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="92"/>
+      <c r="K12" s="116">
         <f>Start!E13</f>
         <v>5</v>
       </c>
-      <c r="L12" s="148"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
-      <c r="O12" s="149"/>
+      <c r="L12" s="117"/>
+      <c r="M12" s="117"/>
+      <c r="N12" s="117"/>
+      <c r="O12" s="118"/>
       <c r="Q12" s="52"/>
-      <c r="R12" s="147">
+      <c r="R12" s="116">
         <f>Start!E11</f>
-        <v>19</v>
-      </c>
-      <c r="S12" s="148"/>
-      <c r="T12" s="148"/>
-      <c r="U12" s="148"/>
-      <c r="V12" s="149"/>
-      <c r="Y12" s="147">
+        <v>17</v>
+      </c>
+      <c r="S12" s="117"/>
+      <c r="T12" s="117"/>
+      <c r="U12" s="117"/>
+      <c r="V12" s="118"/>
+      <c r="Y12" s="116">
         <f>K12+R12</f>
-        <v>24</v>
-      </c>
-      <c r="Z12" s="148"/>
-      <c r="AA12" s="149"/>
+        <v>22</v>
+      </c>
+      <c r="Z12" s="117"/>
+      <c r="AA12" s="118"/>
       <c r="AB12" s="34"/>
       <c r="AC12" s="44"/>
       <c r="AO12" s="53"/>
@@ -3621,36 +3621,36 @@
       <c r="B13" s="47"/>
       <c r="F13" s="55"/>
       <c r="Q13" s="47"/>
-      <c r="R13" s="143" t="s">
+      <c r="R13" s="133" t="s">
         <v>71</v>
       </c>
-      <c r="S13" s="143"/>
-      <c r="T13" s="143"/>
-      <c r="U13" s="143"/>
-      <c r="V13" s="143"/>
-      <c r="Y13" s="138" t="str">
+      <c r="S13" s="133"/>
+      <c r="T13" s="133"/>
+      <c r="U13" s="133"/>
+      <c r="V13" s="133"/>
+      <c r="Y13" s="128" t="str">
         <f>CONCATENATE("verfügbare ",IF(Start!E21="TEILZEIT","Stunden","Urlaubstage"))</f>
         <v>verfügbare Urlaubstage</v>
       </c>
-      <c r="Z13" s="138"/>
-      <c r="AA13" s="138"/>
+      <c r="Z13" s="128"/>
+      <c r="AA13" s="128"/>
       <c r="AB13" s="56"/>
-      <c r="AC13" s="108" t="s">
+      <c r="AC13" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="AD13" s="133" t="s">
+      <c r="AD13" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="AE13" s="133"/>
-      <c r="AF13" s="133"/>
-      <c r="AG13" s="133"/>
-      <c r="AH13" s="133"/>
-      <c r="AI13" s="133"/>
-      <c r="AJ13" s="133"/>
-      <c r="AK13" s="133"/>
-      <c r="AL13" s="133"/>
-      <c r="AM13" s="133"/>
-      <c r="AN13" s="106">
+      <c r="AE13" s="123"/>
+      <c r="AF13" s="123"/>
+      <c r="AG13" s="123"/>
+      <c r="AH13" s="123"/>
+      <c r="AI13" s="123"/>
+      <c r="AJ13" s="123"/>
+      <c r="AK13" s="123"/>
+      <c r="AL13" s="123"/>
+      <c r="AM13" s="123"/>
+      <c r="AN13" s="150">
         <f>IF(COUNTA(R14)=1,1,0)</f>
         <v>1</v>
       </c>
@@ -3658,42 +3658,42 @@
     </row>
     <row r="14" spans="1:51" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="58"/>
-      <c r="B14" s="88" t="s">
+      <c r="B14" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="116"/>
-      <c r="D14" s="116"/>
-      <c r="E14" s="116"/>
-      <c r="F14" s="116"/>
-      <c r="G14" s="116"/>
-      <c r="H14" s="89"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="92"/>
       <c r="Q14" s="52"/>
-      <c r="R14" s="144">
-        <v>0</v>
-      </c>
-      <c r="S14" s="145"/>
-      <c r="T14" s="145"/>
-      <c r="U14" s="145"/>
-      <c r="V14" s="146"/>
-      <c r="Y14" s="120">
+      <c r="R14" s="134">
+        <v>0</v>
+      </c>
+      <c r="S14" s="135"/>
+      <c r="T14" s="135"/>
+      <c r="U14" s="135"/>
+      <c r="V14" s="136"/>
+      <c r="Y14" s="106">
         <f>Y12-R14</f>
-        <v>24</v>
-      </c>
-      <c r="Z14" s="121"/>
-      <c r="AA14" s="122"/>
+        <v>22</v>
+      </c>
+      <c r="Z14" s="107"/>
+      <c r="AA14" s="108"/>
       <c r="AB14" s="59"/>
-      <c r="AC14" s="108"/>
-      <c r="AD14" s="133"/>
-      <c r="AE14" s="133"/>
-      <c r="AF14" s="133"/>
-      <c r="AG14" s="133"/>
-      <c r="AH14" s="133"/>
-      <c r="AI14" s="133"/>
-      <c r="AJ14" s="133"/>
-      <c r="AK14" s="133"/>
-      <c r="AL14" s="133"/>
-      <c r="AM14" s="133"/>
-      <c r="AN14" s="106"/>
+      <c r="AC14" s="110"/>
+      <c r="AD14" s="123"/>
+      <c r="AE14" s="123"/>
+      <c r="AF14" s="123"/>
+      <c r="AG14" s="123"/>
+      <c r="AH14" s="123"/>
+      <c r="AI14" s="123"/>
+      <c r="AJ14" s="123"/>
+      <c r="AK14" s="123"/>
+      <c r="AL14" s="123"/>
+      <c r="AM14" s="123"/>
+      <c r="AN14" s="150"/>
     </row>
     <row r="15" spans="1:51" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="32"/>
@@ -3706,103 +3706,103 @@
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
-      <c r="K15" s="131" t="s">
+      <c r="K15" s="121" t="s">
         <v>30</v>
       </c>
-      <c r="L15" s="132"/>
-      <c r="M15" s="132"/>
-      <c r="N15" s="132"/>
-      <c r="O15" s="132"/>
+      <c r="L15" s="122"/>
+      <c r="M15" s="122"/>
+      <c r="N15" s="122"/>
+      <c r="O15" s="122"/>
       <c r="P15" s="60"/>
       <c r="Q15" s="60"/>
-      <c r="R15" s="131" t="s">
+      <c r="R15" s="121" t="s">
         <v>31</v>
       </c>
-      <c r="S15" s="131"/>
-      <c r="T15" s="132"/>
-      <c r="U15" s="132"/>
-      <c r="V15" s="132"/>
+      <c r="S15" s="121"/>
+      <c r="T15" s="122"/>
+      <c r="U15" s="122"/>
+      <c r="V15" s="122"/>
       <c r="W15" s="35"/>
       <c r="X15" s="35"/>
-      <c r="Y15" s="142" t="str">
+      <c r="Y15" s="132" t="str">
         <f>CONCATENATE("beantragte ",IF(Start!$E$21="TEILZEIT","Stunden","Urlaubstage"))</f>
         <v>beantragte Urlaubstage</v>
       </c>
-      <c r="Z15" s="142"/>
-      <c r="AA15" s="142"/>
+      <c r="Z15" s="132"/>
+      <c r="AA15" s="132"/>
       <c r="AB15" s="61"/>
-      <c r="AC15" s="108" t="s">
+      <c r="AC15" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="AD15" s="133" t="s">
+      <c r="AD15" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="AE15" s="133"/>
-      <c r="AF15" s="133"/>
-      <c r="AG15" s="133"/>
-      <c r="AH15" s="133"/>
-      <c r="AI15" s="133"/>
-      <c r="AJ15" s="133"/>
-      <c r="AK15" s="133"/>
-      <c r="AL15" s="133"/>
-      <c r="AM15" s="133"/>
-      <c r="AN15" s="106">
+      <c r="AE15" s="123"/>
+      <c r="AF15" s="123"/>
+      <c r="AG15" s="123"/>
+      <c r="AH15" s="123"/>
+      <c r="AI15" s="123"/>
+      <c r="AJ15" s="123"/>
+      <c r="AK15" s="123"/>
+      <c r="AL15" s="123"/>
+      <c r="AM15" s="123"/>
+      <c r="AN15" s="150">
         <f>IF(AND(K16&lt;&gt;"",R16&lt;&gt;""),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:51" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="32"/>
-      <c r="B16" s="88" t="s">
+      <c r="B16" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="89"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="115"/>
+      <c r="G16" s="115"/>
+      <c r="H16" s="92"/>
       <c r="I16" s="62"/>
       <c r="J16" s="63"/>
-      <c r="K16" s="117">
+      <c r="K16" s="141">
         <v>42881</v>
       </c>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="119"/>
+      <c r="L16" s="142"/>
+      <c r="M16" s="142"/>
+      <c r="N16" s="142"/>
+      <c r="O16" s="143"/>
       <c r="P16" s="63"/>
       <c r="Q16" s="63"/>
-      <c r="R16" s="117">
+      <c r="R16" s="141">
         <v>42882</v>
       </c>
-      <c r="S16" s="118"/>
-      <c r="T16" s="118"/>
-      <c r="U16" s="118"/>
-      <c r="V16" s="119"/>
+      <c r="S16" s="142"/>
+      <c r="T16" s="142"/>
+      <c r="U16" s="142"/>
+      <c r="V16" s="143"/>
       <c r="X16" s="31">
         <f ca="1">IF(Start!E19&lt;&gt;"",IF(AND(K16&lt;&gt;"",R16&lt;&gt;""),IF(K16&lt;=R16,IF(Start!E21="TEILZEIT",SUM(Frei!H3:H52),NETWORKDAYS(K16,R16)-SUM(Feiertage!D3:D21,Feiertage!L3:L21,Feiertage!T3:T21,Feiertage!AB3:AB21,Feiertage!AJ3:AJ21,Feiertage!AR3:AR21)),"#REIFLG!"),0),0)</f>
         <v>1</v>
       </c>
-      <c r="Y16" s="120">
+      <c r="Y16" s="106">
         <f ca="1">IF(AND(K18="",R18=""),X16,IF(AND(K18&lt;&gt;"",NETWORKDAYS(K16,K16)=1,IFERROR(VLOOKUP(K16,OFFSET(Feiertage!F3,0,Feiertage!A1+YEAR(K16)-2017):OFFSET(Feiertage!F21,0,Feiertage!A1+YEAR(K16)-2017),1,FALSE),FALSE)=FALSE),IF(AND(R18&lt;&gt;"",NETWORKDAYS(R16,R16)=1,IFERROR(VLOOKUP(R16,OFFSET(Feiertage!F3,0,Feiertage!A1+YEAR(R16)-2017):OFFSET(Feiertage!F21,0,Feiertage!A1+YEAR(R16)-2017),1,FALSE),FALSE)=FALSE),X16-1,X16-0.5),IF(AND(R18&lt;&gt;"",NETWORKDAYS(R16,R16)=1,IFERROR(VLOOKUP(R16,OFFSET(Feiertage!F3,0,Feiertage!A1+YEAR(R16)-2017):OFFSET(Feiertage!F21,0,Feiertage!A1+YEAR(R16)-2017),1,FALSE),FALSE)=FALSE),X16-0.5,X16)))</f>
         <v>1</v>
       </c>
-      <c r="Z16" s="121"/>
-      <c r="AA16" s="122"/>
+      <c r="Z16" s="107"/>
+      <c r="AA16" s="108"/>
       <c r="AB16" s="34"/>
-      <c r="AC16" s="108"/>
-      <c r="AD16" s="133"/>
-      <c r="AE16" s="133"/>
-      <c r="AF16" s="133"/>
-      <c r="AG16" s="133"/>
-      <c r="AH16" s="133"/>
-      <c r="AI16" s="133"/>
-      <c r="AJ16" s="133"/>
-      <c r="AK16" s="133"/>
-      <c r="AL16" s="133"/>
-      <c r="AM16" s="133"/>
-      <c r="AN16" s="106"/>
+      <c r="AC16" s="110"/>
+      <c r="AD16" s="123"/>
+      <c r="AE16" s="123"/>
+      <c r="AF16" s="123"/>
+      <c r="AG16" s="123"/>
+      <c r="AH16" s="123"/>
+      <c r="AI16" s="123"/>
+      <c r="AJ16" s="123"/>
+      <c r="AK16" s="123"/>
+      <c r="AL16" s="123"/>
+      <c r="AM16" s="123"/>
+      <c r="AN16" s="150"/>
       <c r="AO16" s="64"/>
     </row>
     <row r="17" spans="1:40" ht="3.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
@@ -3834,22 +3834,22 @@
       <c r="Z17" s="30"/>
       <c r="AA17" s="30"/>
       <c r="AB17" s="65"/>
-      <c r="AC17" s="153" t="s">
+      <c r="AC17" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="AD17" s="86" t="s">
+      <c r="AD17" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="AE17" s="86"/>
-      <c r="AF17" s="86"/>
-      <c r="AG17" s="86"/>
-      <c r="AH17" s="86"/>
-      <c r="AI17" s="86"/>
-      <c r="AJ17" s="86"/>
-      <c r="AK17" s="86"/>
-      <c r="AL17" s="86"/>
-      <c r="AM17" s="86"/>
-      <c r="AN17" s="106">
+      <c r="AE17" s="104"/>
+      <c r="AF17" s="104"/>
+      <c r="AG17" s="104"/>
+      <c r="AH17" s="104"/>
+      <c r="AI17" s="104"/>
+      <c r="AJ17" s="104"/>
+      <c r="AK17" s="104"/>
+      <c r="AL17" s="104"/>
+      <c r="AM17" s="104"/>
+      <c r="AN17" s="150">
         <f ca="1">IF(Start!E21="Teilzeit",1,IF(AND(X16=0,OR(K18&lt;&gt;"",R18&lt;&gt;"",K20&lt;&gt;"",N20&lt;&gt;"",R20&lt;&gt;"",U20&lt;&gt;"")),0,IF(AND(X16=1,OR(R18&lt;&gt;"",R20&lt;&gt;"",U20&lt;&gt;"")),0,IF(AND(K18="",R18=""),IF(AND(K20="",N20="",R20="",U20=""),1,0),IF(AND(K18&lt;&gt;"",R18&lt;&gt;""),IF(AND(OR(K20&lt;&gt;"",N20&lt;&gt;""),OR(R20&lt;&gt;"",U20&lt;&gt;"")),1,0),IF(AND(K18&lt;&gt;"",OR(K20&lt;&gt;"",N20&lt;&gt;"")),1,IF(AND(R18&lt;&gt;"",OR(R20&lt;&gt;"",U20&lt;&gt;"")),1,0)))))))</f>
         <v>1</v>
       </c>
@@ -3866,41 +3866,41 @@
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
       <c r="K18" s="79"/>
-      <c r="L18" s="134" t="s">
+      <c r="L18" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="M18" s="135"/>
-      <c r="N18" s="135"/>
-      <c r="O18" s="135"/>
+      <c r="M18" s="125"/>
+      <c r="N18" s="125"/>
+      <c r="O18" s="125"/>
       <c r="P18" s="30"/>
       <c r="Q18" s="30"/>
       <c r="R18" s="79"/>
-      <c r="S18" s="134" t="s">
+      <c r="S18" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="T18" s="135"/>
-      <c r="U18" s="135"/>
-      <c r="V18" s="135"/>
+      <c r="T18" s="125"/>
+      <c r="U18" s="125"/>
+      <c r="V18" s="125"/>
       <c r="W18" s="30"/>
       <c r="X18" s="30"/>
-      <c r="Y18" s="113" t="s">
+      <c r="Y18" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="Z18" s="113"/>
-      <c r="AA18" s="113"/>
+      <c r="Z18" s="119"/>
+      <c r="AA18" s="119"/>
       <c r="AB18" s="65"/>
-      <c r="AC18" s="153"/>
-      <c r="AD18" s="86"/>
-      <c r="AE18" s="86"/>
-      <c r="AF18" s="86"/>
-      <c r="AG18" s="86"/>
-      <c r="AH18" s="86"/>
-      <c r="AI18" s="86"/>
-      <c r="AJ18" s="86"/>
-      <c r="AK18" s="86"/>
-      <c r="AL18" s="86"/>
-      <c r="AM18" s="86"/>
-      <c r="AN18" s="106"/>
+      <c r="AC18" s="109"/>
+      <c r="AD18" s="104"/>
+      <c r="AE18" s="104"/>
+      <c r="AF18" s="104"/>
+      <c r="AG18" s="104"/>
+      <c r="AH18" s="104"/>
+      <c r="AI18" s="104"/>
+      <c r="AJ18" s="104"/>
+      <c r="AK18" s="104"/>
+      <c r="AL18" s="104"/>
+      <c r="AM18" s="104"/>
+      <c r="AN18" s="150"/>
     </row>
     <row r="19" spans="1:40" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="32"/>
@@ -3927,22 +3927,22 @@
       <c r="V19" s="66"/>
       <c r="W19" s="30"/>
       <c r="X19" s="30"/>
-      <c r="Y19" s="113"/>
-      <c r="Z19" s="113"/>
-      <c r="AA19" s="113"/>
+      <c r="Y19" s="119"/>
+      <c r="Z19" s="119"/>
+      <c r="AA19" s="119"/>
       <c r="AB19" s="65"/>
-      <c r="AC19" s="153"/>
-      <c r="AD19" s="86"/>
-      <c r="AE19" s="86"/>
-      <c r="AF19" s="86"/>
-      <c r="AG19" s="86"/>
-      <c r="AH19" s="86"/>
-      <c r="AI19" s="86"/>
-      <c r="AJ19" s="86"/>
-      <c r="AK19" s="86"/>
-      <c r="AL19" s="86"/>
-      <c r="AM19" s="86"/>
-      <c r="AN19" s="106"/>
+      <c r="AC19" s="109"/>
+      <c r="AD19" s="104"/>
+      <c r="AE19" s="104"/>
+      <c r="AF19" s="104"/>
+      <c r="AG19" s="104"/>
+      <c r="AH19" s="104"/>
+      <c r="AI19" s="104"/>
+      <c r="AJ19" s="104"/>
+      <c r="AK19" s="104"/>
+      <c r="AL19" s="104"/>
+      <c r="AM19" s="104"/>
+      <c r="AN19" s="150"/>
     </row>
     <row r="20" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="32"/>
@@ -3977,22 +3977,22 @@
       </c>
       <c r="W20" s="30"/>
       <c r="X20" s="30"/>
-      <c r="Y20" s="113"/>
-      <c r="Z20" s="113"/>
-      <c r="AA20" s="113"/>
+      <c r="Y20" s="119"/>
+      <c r="Z20" s="119"/>
+      <c r="AA20" s="119"/>
       <c r="AB20" s="65"/>
-      <c r="AC20" s="153"/>
-      <c r="AD20" s="86"/>
-      <c r="AE20" s="86"/>
-      <c r="AF20" s="86"/>
-      <c r="AG20" s="86"/>
-      <c r="AH20" s="86"/>
-      <c r="AI20" s="86"/>
-      <c r="AJ20" s="86"/>
-      <c r="AK20" s="86"/>
-      <c r="AL20" s="86"/>
-      <c r="AM20" s="86"/>
-      <c r="AN20" s="106"/>
+      <c r="AC20" s="109"/>
+      <c r="AD20" s="104"/>
+      <c r="AE20" s="104"/>
+      <c r="AF20" s="104"/>
+      <c r="AG20" s="104"/>
+      <c r="AH20" s="104"/>
+      <c r="AI20" s="104"/>
+      <c r="AJ20" s="104"/>
+      <c r="AK20" s="104"/>
+      <c r="AL20" s="104"/>
+      <c r="AM20" s="104"/>
+      <c r="AN20" s="150"/>
     </row>
     <row r="21" spans="1:40" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="32"/>
@@ -4007,76 +4007,76 @@
       <c r="J21" s="30"/>
       <c r="W21" s="30"/>
       <c r="X21" s="30"/>
-      <c r="Y21" s="114"/>
-      <c r="Z21" s="114"/>
-      <c r="AA21" s="114"/>
+      <c r="Y21" s="139"/>
+      <c r="Z21" s="139"/>
+      <c r="AA21" s="139"/>
       <c r="AB21" s="34"/>
-      <c r="AC21" s="153" t="s">
+      <c r="AC21" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="AD21" s="110" t="s">
+      <c r="AD21" s="153" t="s">
         <v>84</v>
       </c>
-      <c r="AE21" s="110"/>
-      <c r="AF21" s="110"/>
-      <c r="AG21" s="110"/>
-      <c r="AH21" s="110"/>
-      <c r="AI21" s="110"/>
-      <c r="AJ21" s="110"/>
-      <c r="AK21" s="110"/>
-      <c r="AL21" s="110"/>
-      <c r="AM21" s="110"/>
-      <c r="AN21" s="106"/>
+      <c r="AE21" s="153"/>
+      <c r="AF21" s="153"/>
+      <c r="AG21" s="153"/>
+      <c r="AH21" s="153"/>
+      <c r="AI21" s="153"/>
+      <c r="AJ21" s="153"/>
+      <c r="AK21" s="153"/>
+      <c r="AL21" s="153"/>
+      <c r="AM21" s="153"/>
+      <c r="AN21" s="150"/>
     </row>
     <row r="22" spans="1:40" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="32"/>
-      <c r="B22" s="88" t="s">
+      <c r="B22" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="116"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="89"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="92"/>
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
-      <c r="K22" s="136" t="str">
+      <c r="K22" s="126" t="str">
         <f ca="1">IF(AND(K16&lt;&gt;"",R16&lt;&gt;""),IF(Frei!A1&lt;&gt;"",CONCATENATE("Incl. Feiertage: ",IF(LEN(Frei!A1)&gt;70,CONCATENATE(MID(Frei!A1,1,70),"…"),Frei!A1)),""),"")</f>
         <v/>
       </c>
-      <c r="L22" s="136"/>
-      <c r="M22" s="136"/>
-      <c r="N22" s="136"/>
-      <c r="O22" s="136"/>
-      <c r="P22" s="136"/>
-      <c r="Q22" s="136"/>
-      <c r="R22" s="136"/>
-      <c r="S22" s="136"/>
-      <c r="T22" s="136"/>
-      <c r="U22" s="136"/>
-      <c r="V22" s="136"/>
+      <c r="L22" s="126"/>
+      <c r="M22" s="126"/>
+      <c r="N22" s="126"/>
+      <c r="O22" s="126"/>
+      <c r="P22" s="126"/>
+      <c r="Q22" s="126"/>
+      <c r="R22" s="126"/>
+      <c r="S22" s="126"/>
+      <c r="T22" s="126"/>
+      <c r="U22" s="126"/>
+      <c r="V22" s="126"/>
       <c r="W22" s="67"/>
       <c r="X22" s="67"/>
-      <c r="Y22" s="139">
+      <c r="Y22" s="129">
         <f ca="1">IF(Y16="#REIFLG!",Y14,Y14-Y16)</f>
-        <v>23</v>
-      </c>
-      <c r="Z22" s="140"/>
-      <c r="AA22" s="141"/>
+        <v>21</v>
+      </c>
+      <c r="Z22" s="130"/>
+      <c r="AA22" s="131"/>
       <c r="AB22" s="68"/>
-      <c r="AC22" s="153"/>
-      <c r="AD22" s="110"/>
-      <c r="AE22" s="110"/>
-      <c r="AF22" s="110"/>
-      <c r="AG22" s="110"/>
-      <c r="AH22" s="110"/>
-      <c r="AI22" s="110"/>
-      <c r="AJ22" s="110"/>
-      <c r="AK22" s="110"/>
-      <c r="AL22" s="110"/>
-      <c r="AM22" s="110"/>
-      <c r="AN22" s="106"/>
+      <c r="AC22" s="109"/>
+      <c r="AD22" s="153"/>
+      <c r="AE22" s="153"/>
+      <c r="AF22" s="153"/>
+      <c r="AG22" s="153"/>
+      <c r="AH22" s="153"/>
+      <c r="AI22" s="153"/>
+      <c r="AJ22" s="153"/>
+      <c r="AK22" s="153"/>
+      <c r="AL22" s="153"/>
+      <c r="AM22" s="153"/>
+      <c r="AN22" s="150"/>
     </row>
     <row r="23" spans="1:40" ht="7.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A23" s="32"/>
@@ -4107,62 +4107,62 @@
       <c r="Z23" s="72"/>
       <c r="AA23" s="72"/>
       <c r="AB23" s="68"/>
-      <c r="AC23" s="108"/>
-      <c r="AD23" s="109"/>
-      <c r="AE23" s="109"/>
-      <c r="AF23" s="109"/>
-      <c r="AG23" s="109"/>
-      <c r="AH23" s="109"/>
-      <c r="AI23" s="109"/>
-      <c r="AJ23" s="109"/>
-      <c r="AK23" s="109"/>
-      <c r="AL23" s="109"/>
-      <c r="AM23" s="109"/>
-      <c r="AN23" s="106"/>
+      <c r="AC23" s="110"/>
+      <c r="AD23" s="152"/>
+      <c r="AE23" s="152"/>
+      <c r="AF23" s="152"/>
+      <c r="AG23" s="152"/>
+      <c r="AH23" s="152"/>
+      <c r="AI23" s="152"/>
+      <c r="AJ23" s="152"/>
+      <c r="AK23" s="152"/>
+      <c r="AL23" s="152"/>
+      <c r="AM23" s="152"/>
+      <c r="AN23" s="150"/>
     </row>
     <row r="24" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="32"/>
-      <c r="B24" s="112" t="s">
+      <c r="B24" s="138" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="112"/>
+      <c r="C24" s="138"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="138"/>
       <c r="I24" s="38"/>
       <c r="J24" s="35"/>
-      <c r="K24" s="137"/>
-      <c r="L24" s="137"/>
-      <c r="M24" s="137"/>
-      <c r="N24" s="137"/>
-      <c r="O24" s="137"/>
-      <c r="P24" s="137"/>
-      <c r="Q24" s="137"/>
-      <c r="R24" s="137"/>
-      <c r="S24" s="137"/>
-      <c r="T24" s="137"/>
-      <c r="U24" s="137"/>
-      <c r="V24" s="137"/>
-      <c r="W24" s="137"/>
-      <c r="X24" s="137"/>
-      <c r="Y24" s="137"/>
-      <c r="Z24" s="137"/>
-      <c r="AA24" s="137"/>
+      <c r="K24" s="127"/>
+      <c r="L24" s="127"/>
+      <c r="M24" s="127"/>
+      <c r="N24" s="127"/>
+      <c r="O24" s="127"/>
+      <c r="P24" s="127"/>
+      <c r="Q24" s="127"/>
+      <c r="R24" s="127"/>
+      <c r="S24" s="127"/>
+      <c r="T24" s="127"/>
+      <c r="U24" s="127"/>
+      <c r="V24" s="127"/>
+      <c r="W24" s="127"/>
+      <c r="X24" s="127"/>
+      <c r="Y24" s="127"/>
+      <c r="Z24" s="127"/>
+      <c r="AA24" s="127"/>
       <c r="AB24" s="65"/>
-      <c r="AC24" s="108"/>
-      <c r="AD24" s="109"/>
-      <c r="AE24" s="109"/>
-      <c r="AF24" s="109"/>
-      <c r="AG24" s="109"/>
-      <c r="AH24" s="109"/>
-      <c r="AI24" s="109"/>
-      <c r="AJ24" s="109"/>
-      <c r="AK24" s="109"/>
-      <c r="AL24" s="109"/>
-      <c r="AM24" s="109"/>
-      <c r="AN24" s="106"/>
+      <c r="AC24" s="110"/>
+      <c r="AD24" s="152"/>
+      <c r="AE24" s="152"/>
+      <c r="AF24" s="152"/>
+      <c r="AG24" s="152"/>
+      <c r="AH24" s="152"/>
+      <c r="AI24" s="152"/>
+      <c r="AJ24" s="152"/>
+      <c r="AK24" s="152"/>
+      <c r="AL24" s="152"/>
+      <c r="AM24" s="152"/>
+      <c r="AN24" s="150"/>
     </row>
     <row r="25" spans="1:40" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="32"/>
@@ -4191,18 +4191,18 @@
       <c r="Z25" s="30"/>
       <c r="AA25" s="30"/>
       <c r="AB25" s="65"/>
-      <c r="AC25" s="108"/>
-      <c r="AD25" s="109"/>
-      <c r="AE25" s="109"/>
-      <c r="AF25" s="109"/>
-      <c r="AG25" s="109"/>
-      <c r="AH25" s="109"/>
-      <c r="AI25" s="109"/>
-      <c r="AJ25" s="109"/>
-      <c r="AK25" s="109"/>
-      <c r="AL25" s="109"/>
-      <c r="AM25" s="109"/>
-      <c r="AN25" s="106"/>
+      <c r="AC25" s="110"/>
+      <c r="AD25" s="152"/>
+      <c r="AE25" s="152"/>
+      <c r="AF25" s="152"/>
+      <c r="AG25" s="152"/>
+      <c r="AH25" s="152"/>
+      <c r="AI25" s="152"/>
+      <c r="AJ25" s="152"/>
+      <c r="AK25" s="152"/>
+      <c r="AL25" s="152"/>
+      <c r="AM25" s="152"/>
+      <c r="AN25" s="150"/>
     </row>
     <row r="26" spans="1:40" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="32"/>
@@ -4233,22 +4233,22 @@
       <c r="Z26" s="35"/>
       <c r="AA26" s="35"/>
       <c r="AB26" s="34"/>
-      <c r="AC26" s="108" t="s">
+      <c r="AC26" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="AD26" s="86" t="s">
+      <c r="AD26" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="AE26" s="86"/>
-      <c r="AF26" s="86"/>
-      <c r="AG26" s="86"/>
-      <c r="AH26" s="86"/>
-      <c r="AI26" s="86"/>
-      <c r="AJ26" s="86"/>
-      <c r="AK26" s="86"/>
-      <c r="AL26" s="86"/>
-      <c r="AM26" s="86"/>
-      <c r="AN26" s="106">
+      <c r="AE26" s="104"/>
+      <c r="AF26" s="104"/>
+      <c r="AG26" s="104"/>
+      <c r="AH26" s="104"/>
+      <c r="AI26" s="104"/>
+      <c r="AJ26" s="104"/>
+      <c r="AK26" s="104"/>
+      <c r="AL26" s="104"/>
+      <c r="AM26" s="104"/>
+      <c r="AN26" s="150">
         <f>IF(R27&lt;&gt;"",1,0)</f>
         <v>1</v>
       </c>
@@ -4273,31 +4273,31 @@
       <c r="O27" s="35"/>
       <c r="P27" s="35"/>
       <c r="Q27" s="35"/>
-      <c r="R27" s="151" t="s">
+      <c r="R27" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="S27" s="151"/>
-      <c r="T27" s="151"/>
-      <c r="U27" s="151"/>
-      <c r="V27" s="151"/>
-      <c r="W27" s="151"/>
-      <c r="X27" s="151"/>
-      <c r="Y27" s="151"/>
-      <c r="Z27" s="151"/>
-      <c r="AA27" s="151"/>
+      <c r="S27" s="111"/>
+      <c r="T27" s="111"/>
+      <c r="U27" s="111"/>
+      <c r="V27" s="111"/>
+      <c r="W27" s="111"/>
+      <c r="X27" s="111"/>
+      <c r="Y27" s="111"/>
+      <c r="Z27" s="111"/>
+      <c r="AA27" s="111"/>
       <c r="AB27" s="34"/>
-      <c r="AC27" s="108"/>
-      <c r="AD27" s="86"/>
-      <c r="AE27" s="86"/>
-      <c r="AF27" s="86"/>
-      <c r="AG27" s="86"/>
-      <c r="AH27" s="86"/>
-      <c r="AI27" s="86"/>
-      <c r="AJ27" s="86"/>
-      <c r="AK27" s="86"/>
-      <c r="AL27" s="86"/>
-      <c r="AM27" s="86"/>
-      <c r="AN27" s="106"/>
+      <c r="AC27" s="110"/>
+      <c r="AD27" s="104"/>
+      <c r="AE27" s="104"/>
+      <c r="AF27" s="104"/>
+      <c r="AG27" s="104"/>
+      <c r="AH27" s="104"/>
+      <c r="AI27" s="104"/>
+      <c r="AJ27" s="104"/>
+      <c r="AK27" s="104"/>
+      <c r="AL27" s="104"/>
+      <c r="AM27" s="104"/>
+      <c r="AN27" s="150"/>
     </row>
     <row r="28" spans="1:40" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="32"/>
@@ -4328,22 +4328,22 @@
       <c r="Z28" s="35"/>
       <c r="AA28" s="35"/>
       <c r="AB28" s="34"/>
-      <c r="AC28" s="108" t="s">
+      <c r="AC28" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="AD28" s="86" t="s">
+      <c r="AD28" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="AE28" s="86"/>
-      <c r="AF28" s="86"/>
-      <c r="AG28" s="86"/>
-      <c r="AH28" s="86"/>
-      <c r="AI28" s="86"/>
-      <c r="AJ28" s="86"/>
-      <c r="AK28" s="86"/>
-      <c r="AL28" s="86"/>
-      <c r="AM28" s="86"/>
-      <c r="AN28" s="106"/>
+      <c r="AE28" s="104"/>
+      <c r="AF28" s="104"/>
+      <c r="AG28" s="104"/>
+      <c r="AH28" s="104"/>
+      <c r="AI28" s="104"/>
+      <c r="AJ28" s="104"/>
+      <c r="AK28" s="104"/>
+      <c r="AL28" s="104"/>
+      <c r="AM28" s="104"/>
+      <c r="AN28" s="150"/>
     </row>
     <row r="29" spans="1:40" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="32"/>
@@ -4365,29 +4365,29 @@
       <c r="O29" s="35"/>
       <c r="P29" s="35"/>
       <c r="Q29" s="35"/>
-      <c r="R29" s="152"/>
-      <c r="S29" s="152"/>
-      <c r="T29" s="152"/>
-      <c r="U29" s="152"/>
-      <c r="V29" s="152"/>
-      <c r="W29" s="152"/>
-      <c r="X29" s="152"/>
-      <c r="Y29" s="152"/>
-      <c r="Z29" s="152"/>
-      <c r="AA29" s="152"/>
+      <c r="R29" s="112"/>
+      <c r="S29" s="112"/>
+      <c r="T29" s="112"/>
+      <c r="U29" s="112"/>
+      <c r="V29" s="112"/>
+      <c r="W29" s="112"/>
+      <c r="X29" s="112"/>
+      <c r="Y29" s="112"/>
+      <c r="Z29" s="112"/>
+      <c r="AA29" s="112"/>
       <c r="AB29" s="34"/>
-      <c r="AC29" s="108"/>
-      <c r="AD29" s="86"/>
-      <c r="AE29" s="86"/>
-      <c r="AF29" s="86"/>
-      <c r="AG29" s="86"/>
-      <c r="AH29" s="86"/>
-      <c r="AI29" s="86"/>
-      <c r="AJ29" s="86"/>
-      <c r="AK29" s="86"/>
-      <c r="AL29" s="86"/>
-      <c r="AM29" s="86"/>
-      <c r="AN29" s="106"/>
+      <c r="AC29" s="110"/>
+      <c r="AD29" s="104"/>
+      <c r="AE29" s="104"/>
+      <c r="AF29" s="104"/>
+      <c r="AG29" s="104"/>
+      <c r="AH29" s="104"/>
+      <c r="AI29" s="104"/>
+      <c r="AJ29" s="104"/>
+      <c r="AK29" s="104"/>
+      <c r="AL29" s="104"/>
+      <c r="AM29" s="104"/>
+      <c r="AN29" s="150"/>
     </row>
     <row r="30" spans="1:40" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="32"/>
@@ -4418,19 +4418,19 @@
       <c r="Z30" s="35"/>
       <c r="AA30" s="35"/>
       <c r="AB30" s="34"/>
-      <c r="AD30" s="86" t="s">
+      <c r="AD30" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="AE30" s="86"/>
-      <c r="AF30" s="86"/>
-      <c r="AG30" s="86"/>
-      <c r="AH30" s="86"/>
-      <c r="AI30" s="86"/>
-      <c r="AJ30" s="86"/>
-      <c r="AK30" s="86"/>
-      <c r="AL30" s="86"/>
-      <c r="AM30" s="86"/>
-      <c r="AN30" s="106"/>
+      <c r="AE30" s="104"/>
+      <c r="AF30" s="104"/>
+      <c r="AG30" s="104"/>
+      <c r="AH30" s="104"/>
+      <c r="AI30" s="104"/>
+      <c r="AJ30" s="104"/>
+      <c r="AK30" s="104"/>
+      <c r="AL30" s="104"/>
+      <c r="AM30" s="104"/>
+      <c r="AN30" s="150"/>
     </row>
     <row r="31" spans="1:40" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="32"/>
@@ -4452,31 +4452,31 @@
       <c r="O31" s="35"/>
       <c r="P31" s="35"/>
       <c r="Q31" s="35"/>
-      <c r="R31" s="130"/>
-      <c r="S31" s="130"/>
-      <c r="T31" s="130"/>
-      <c r="U31" s="130"/>
-      <c r="V31" s="130"/>
-      <c r="W31" s="130"/>
-      <c r="X31" s="130"/>
-      <c r="Y31" s="130"/>
-      <c r="Z31" s="130"/>
-      <c r="AA31" s="130"/>
+      <c r="R31" s="113"/>
+      <c r="S31" s="113"/>
+      <c r="T31" s="113"/>
+      <c r="U31" s="113"/>
+      <c r="V31" s="113"/>
+      <c r="W31" s="113"/>
+      <c r="X31" s="113"/>
+      <c r="Y31" s="113"/>
+      <c r="Z31" s="113"/>
+      <c r="AA31" s="113"/>
       <c r="AB31" s="34"/>
       <c r="AC31" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="AD31" s="86"/>
-      <c r="AE31" s="86"/>
-      <c r="AF31" s="86"/>
-      <c r="AG31" s="86"/>
-      <c r="AH31" s="86"/>
-      <c r="AI31" s="86"/>
-      <c r="AJ31" s="86"/>
-      <c r="AK31" s="86"/>
-      <c r="AL31" s="86"/>
-      <c r="AM31" s="86"/>
-      <c r="AN31" s="106"/>
+      <c r="AD31" s="104"/>
+      <c r="AE31" s="104"/>
+      <c r="AF31" s="104"/>
+      <c r="AG31" s="104"/>
+      <c r="AH31" s="104"/>
+      <c r="AI31" s="104"/>
+      <c r="AJ31" s="104"/>
+      <c r="AK31" s="104"/>
+      <c r="AL31" s="104"/>
+      <c r="AM31" s="104"/>
+      <c r="AN31" s="150"/>
     </row>
     <row r="32" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="32"/>
@@ -4507,19 +4507,19 @@
       <c r="Z32" s="35"/>
       <c r="AA32" s="35"/>
       <c r="AB32" s="34"/>
-      <c r="AD32" s="133" t="s">
+      <c r="AD32" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="AE32" s="133"/>
-      <c r="AF32" s="133"/>
-      <c r="AG32" s="133"/>
-      <c r="AH32" s="133"/>
-      <c r="AI32" s="133"/>
-      <c r="AJ32" s="133"/>
-      <c r="AK32" s="133"/>
-      <c r="AL32" s="133"/>
-      <c r="AM32" s="133"/>
-      <c r="AN32" s="106"/>
+      <c r="AE32" s="123"/>
+      <c r="AF32" s="123"/>
+      <c r="AG32" s="123"/>
+      <c r="AH32" s="123"/>
+      <c r="AI32" s="123"/>
+      <c r="AJ32" s="123"/>
+      <c r="AK32" s="123"/>
+      <c r="AL32" s="123"/>
+      <c r="AM32" s="123"/>
+      <c r="AN32" s="150"/>
     </row>
     <row r="33" spans="1:40" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="32"/>
@@ -4541,31 +4541,31 @@
       <c r="O33" s="35"/>
       <c r="P33" s="35"/>
       <c r="Q33" s="35"/>
-      <c r="R33" s="130"/>
-      <c r="S33" s="130"/>
-      <c r="T33" s="130"/>
-      <c r="U33" s="130"/>
-      <c r="V33" s="130"/>
-      <c r="W33" s="130"/>
-      <c r="X33" s="130"/>
-      <c r="Y33" s="130"/>
-      <c r="Z33" s="130"/>
-      <c r="AA33" s="130"/>
+      <c r="R33" s="113"/>
+      <c r="S33" s="113"/>
+      <c r="T33" s="113"/>
+      <c r="U33" s="113"/>
+      <c r="V33" s="113"/>
+      <c r="W33" s="113"/>
+      <c r="X33" s="113"/>
+      <c r="Y33" s="113"/>
+      <c r="Z33" s="113"/>
+      <c r="AA33" s="113"/>
       <c r="AB33" s="34"/>
       <c r="AC33" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="AD33" s="133"/>
-      <c r="AE33" s="133"/>
-      <c r="AF33" s="133"/>
-      <c r="AG33" s="133"/>
-      <c r="AH33" s="133"/>
-      <c r="AI33" s="133"/>
-      <c r="AJ33" s="133"/>
-      <c r="AK33" s="133"/>
-      <c r="AL33" s="133"/>
-      <c r="AM33" s="133"/>
-      <c r="AN33" s="106"/>
+      <c r="AD33" s="123"/>
+      <c r="AE33" s="123"/>
+      <c r="AF33" s="123"/>
+      <c r="AG33" s="123"/>
+      <c r="AH33" s="123"/>
+      <c r="AI33" s="123"/>
+      <c r="AJ33" s="123"/>
+      <c r="AK33" s="123"/>
+      <c r="AL33" s="123"/>
+      <c r="AM33" s="123"/>
+      <c r="AN33" s="150"/>
     </row>
     <row r="34" spans="1:40" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="75"/>
@@ -4600,24 +4600,38 @@
   </sheetData>
   <sheetProtection password="EBDE" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="66">
-    <mergeCell ref="Y16:AA16"/>
-    <mergeCell ref="AC21:AC22"/>
-    <mergeCell ref="AC17:AC20"/>
-    <mergeCell ref="AC26:AC27"/>
-    <mergeCell ref="AC15:AC16"/>
-    <mergeCell ref="AD28:AM29"/>
-    <mergeCell ref="AD26:AM27"/>
-    <mergeCell ref="R27:AA27"/>
-    <mergeCell ref="R29:AA29"/>
-    <mergeCell ref="R31:AA31"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="K12:O12"/>
-    <mergeCell ref="R12:V12"/>
-    <mergeCell ref="Y12:AA12"/>
-    <mergeCell ref="R11:V11"/>
-    <mergeCell ref="K11:O11"/>
-    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="AN32:AN33"/>
+    <mergeCell ref="AN15:AN16"/>
+    <mergeCell ref="AD8:AM10"/>
+    <mergeCell ref="AC13:AC14"/>
+    <mergeCell ref="AN13:AN14"/>
+    <mergeCell ref="AC28:AC29"/>
+    <mergeCell ref="AC23:AC25"/>
+    <mergeCell ref="AD23:AM25"/>
+    <mergeCell ref="AN23:AN25"/>
+    <mergeCell ref="AN28:AN29"/>
+    <mergeCell ref="AN30:AN31"/>
+    <mergeCell ref="AN26:AN27"/>
+    <mergeCell ref="AD21:AM22"/>
+    <mergeCell ref="AD17:AM20"/>
+    <mergeCell ref="AN17:AN20"/>
+    <mergeCell ref="AN21:AN22"/>
+    <mergeCell ref="AD5:AM7"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="Y18:AA21"/>
+    <mergeCell ref="AD2:AM3"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="K16:O16"/>
+    <mergeCell ref="R16:V16"/>
+    <mergeCell ref="Y14:AA14"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B2:AA3"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="K7:AA7"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="K9:Q9"/>
+    <mergeCell ref="R9:AA9"/>
     <mergeCell ref="R33:AA33"/>
     <mergeCell ref="K15:O15"/>
     <mergeCell ref="AD13:AM14"/>
@@ -4634,38 +4648,24 @@
     <mergeCell ref="R14:V14"/>
     <mergeCell ref="L18:O18"/>
     <mergeCell ref="AD30:AM31"/>
-    <mergeCell ref="AD5:AM7"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="Y18:AA21"/>
-    <mergeCell ref="AD2:AM3"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="K16:O16"/>
-    <mergeCell ref="R16:V16"/>
-    <mergeCell ref="Y14:AA14"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B2:AA3"/>
-    <mergeCell ref="B7:J7"/>
-    <mergeCell ref="K7:AA7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="K9:Q9"/>
-    <mergeCell ref="R9:AA9"/>
-    <mergeCell ref="AN32:AN33"/>
-    <mergeCell ref="AN15:AN16"/>
-    <mergeCell ref="AD8:AM10"/>
-    <mergeCell ref="AC13:AC14"/>
-    <mergeCell ref="AN13:AN14"/>
-    <mergeCell ref="AC28:AC29"/>
-    <mergeCell ref="AC23:AC25"/>
-    <mergeCell ref="AD23:AM25"/>
-    <mergeCell ref="AN23:AN25"/>
-    <mergeCell ref="AN28:AN29"/>
-    <mergeCell ref="AN30:AN31"/>
-    <mergeCell ref="AN26:AN27"/>
-    <mergeCell ref="AD21:AM22"/>
-    <mergeCell ref="AD17:AM20"/>
-    <mergeCell ref="AN17:AN20"/>
-    <mergeCell ref="AN21:AN22"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="R12:V12"/>
+    <mergeCell ref="Y12:AA12"/>
+    <mergeCell ref="R11:V11"/>
+    <mergeCell ref="K11:O11"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="AD28:AM29"/>
+    <mergeCell ref="AD26:AM27"/>
+    <mergeCell ref="R27:AA27"/>
+    <mergeCell ref="R29:AA29"/>
+    <mergeCell ref="R31:AA31"/>
+    <mergeCell ref="Y16:AA16"/>
+    <mergeCell ref="AC21:AC22"/>
+    <mergeCell ref="AC17:AC20"/>
+    <mergeCell ref="AC26:AC27"/>
+    <mergeCell ref="AC15:AC16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="R14:S14 R27:S27 K16:O16 R12:V12 R16:V16 K7:AA7 K12:O12">

</xml_diff>